<commit_message>
tried a model with two geological units Peter and JC helped
</commit_message>
<xml_diff>
--- a/trials_waiwera/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
+++ b/trials_waiwera/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/minc/minc_5_spot/plotd_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials_waiwera/minc/minc_5_spot/plotd_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1018" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{548525E2-9AB4-4E2B-97BC-3403A498F387}"/>
+  <xr:revisionPtr revIDLastSave="1020" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBDF93A8-DF37-4D20-AE1C-89DC5FE08807}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7715,7 +7715,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$L$15</c15:sqref>
@@ -7756,7 +7756,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$K$16:$K$27</c15:sqref>
@@ -7807,7 +7807,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$L$16:$L$27</c15:sqref>
@@ -7857,7 +7857,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-8187-4A7A-82B3-4856B8504CC0}"/>
                   </c:ext>
@@ -7870,7 +7870,7 @@
                 <c:order val="18"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$V$15</c15:sqref>
@@ -7912,7 +7912,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$U$16:$U$27</c15:sqref>
@@ -7963,7 +7963,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$V$16:$V$27</c15:sqref>
@@ -8013,7 +8013,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-8187-4A7A-82B3-4856B8504CC0}"/>
                   </c:ext>
@@ -8901,7 +8901,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$H$1</c15:sqref>
@@ -8943,7 +8943,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$G$2:$G$12</c15:sqref>
@@ -8991,7 +8991,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$H$2:$H$12</c15:sqref>
@@ -9038,7 +9038,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-8187-4A7A-82B3-4856B8504CC0}"/>
                   </c:ext>
@@ -9051,7 +9051,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$L$1</c15:sqref>
@@ -9093,7 +9093,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$K$2:$K$14</c15:sqref>
@@ -9144,7 +9144,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$L$2:$L$13</c15:sqref>
@@ -9194,7 +9194,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-8187-4A7A-82B3-4856B8504CC0}"/>
                   </c:ext>
@@ -9207,7 +9207,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$R$1</c15:sqref>
@@ -9254,7 +9254,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$Q$2:$Q$12</c15:sqref>
@@ -9302,7 +9302,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$R$2:$R$12</c15:sqref>
@@ -9349,7 +9349,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-8187-4A7A-82B3-4856B8504CC0}"/>
                   </c:ext>
@@ -9362,7 +9362,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$V$1</c15:sqref>
@@ -9409,7 +9409,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$U$2:$U$13</c15:sqref>
@@ -9460,7 +9460,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$V$2:$V$13</c15:sqref>
@@ -9510,7 +9510,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000011-8187-4A7A-82B3-4856B8504CC0}"/>
                   </c:ext>
@@ -9523,7 +9523,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$AB$1</c15:sqref>
@@ -9570,7 +9570,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$AA$2:$AA$12</c15:sqref>
@@ -9618,7 +9618,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>validation!$AB$2:$AB$12</c15:sqref>
@@ -9665,7 +9665,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000014-8187-4A7A-82B3-4856B8504CC0}"/>
                   </c:ext>
@@ -17551,16 +17551,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>681036</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20644,8 +20644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C03297-68D1-4CBC-9F09-124F29CED069}">
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S45" workbookViewId="0">
-      <selection activeCell="Y68" sqref="Y68"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>